<commit_message>
New feature: Remove duplicate question
</commit_message>
<xml_diff>
--- a/data/SearchData.xlsx
+++ b/data/SearchData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/share/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baohoang/Python/ExcelProcessing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF46C4B4-23FF-2945-9E81-6DF84EE5836F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD3CC6A-5947-B741-A2FF-60508A880053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="600" windowWidth="14240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28700" yWindow="4200" windowWidth="28600" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BỘ CÂU HỎI ÔN TẬP" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="2975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3337" uniqueCount="2975">
   <si>
     <t>CÂU HỎI</t>
   </si>
@@ -11180,10 +11180,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G698"/>
+  <dimension ref="A1:G699"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B189" sqref="B189"/>
+    <sheetView tabSelected="1" topLeftCell="A689" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B703" sqref="B703"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -11282,7 +11282,7 @@
       <c r="F8" s="140"/>
       <c r="G8" s="140"/>
     </row>
-    <row r="9" spans="1:7" ht="38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="57" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>9</v>
       </c>
@@ -11305,7 +11305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="133" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="152" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>1</v>
       </c>
@@ -11855,7 +11855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="57" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="76" x14ac:dyDescent="0.25">
       <c r="A34" s="30">
         <v>25</v>
       </c>
@@ -12096,7 +12096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="57" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="76" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
         <v>36</v>
       </c>
@@ -12293,7 +12293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="57" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="76" x14ac:dyDescent="0.25">
       <c r="A54" s="30">
         <v>45</v>
       </c>
@@ -12680,7 +12680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="133" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="152" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
         <v>62</v>
       </c>
@@ -26899,6 +26899,29 @@
         <v>2960</v>
       </c>
       <c r="G698" s="4" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="699" spans="1:7" ht="38" x14ac:dyDescent="0.25">
+      <c r="A699" s="129">
+        <v>100</v>
+      </c>
+      <c r="B699" s="15" t="s">
+        <v>2956</v>
+      </c>
+      <c r="C699" s="59" t="s">
+        <v>2957</v>
+      </c>
+      <c r="D699" s="4" t="s">
+        <v>2958</v>
+      </c>
+      <c r="E699" s="4" t="s">
+        <v>2959</v>
+      </c>
+      <c r="F699" s="4" t="s">
+        <v>2960</v>
+      </c>
+      <c r="G699" s="4" t="s">
         <v>883</v>
       </c>
     </row>

</xml_diff>